<commit_message>
finished running all experiments
</commit_message>
<xml_diff>
--- a/M0.4D0.0001E0.5A0.8_100x100_MC25_table_experiment.xlsx
+++ b/M0.4D0.0001E0.5A0.8_100x100_MC25_table_experiment.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G161"/>
+  <dimension ref="A1:G201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4470,6 +4470,1006 @@
         <v>0.7951</v>
       </c>
     </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>2598</v>
+      </c>
+      <c r="B162" t="n">
+        <v>24999</v>
+      </c>
+      <c r="C162" t="n">
+        <v>1</v>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>[3158]</t>
+        </is>
+      </c>
+      <c r="E162" t="n">
+        <v>3158</v>
+      </c>
+      <c r="F162" t="n">
+        <v>3941</v>
+      </c>
+      <c r="G162" t="n">
+        <v>0.8013</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>2599</v>
+      </c>
+      <c r="B163" t="n">
+        <v>224999</v>
+      </c>
+      <c r="C163" t="n">
+        <v>1</v>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>[3257]</t>
+        </is>
+      </c>
+      <c r="E163" t="n">
+        <v>3257</v>
+      </c>
+      <c r="F163" t="n">
+        <v>4118</v>
+      </c>
+      <c r="G163" t="n">
+        <v>0.7909</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>2600</v>
+      </c>
+      <c r="B164" t="n">
+        <v>1649999</v>
+      </c>
+      <c r="C164" t="n">
+        <v>1</v>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>[3223]</t>
+        </is>
+      </c>
+      <c r="E164" t="n">
+        <v>3223</v>
+      </c>
+      <c r="F164" t="n">
+        <v>4024</v>
+      </c>
+      <c r="G164" t="n">
+        <v>0.8008999999999999</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>2601</v>
+      </c>
+      <c r="B165" t="n">
+        <v>199999</v>
+      </c>
+      <c r="C165" t="n">
+        <v>1</v>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>[3208]</t>
+        </is>
+      </c>
+      <c r="E165" t="n">
+        <v>3208</v>
+      </c>
+      <c r="F165" t="n">
+        <v>4043</v>
+      </c>
+      <c r="G165" t="n">
+        <v>0.7935</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>2602</v>
+      </c>
+      <c r="B166" t="n">
+        <v>924999</v>
+      </c>
+      <c r="C166" t="n">
+        <v>1</v>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>[3233]</t>
+        </is>
+      </c>
+      <c r="E166" t="n">
+        <v>3233</v>
+      </c>
+      <c r="F166" t="n">
+        <v>4027</v>
+      </c>
+      <c r="G166" t="n">
+        <v>0.8028</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>2603</v>
+      </c>
+      <c r="B167" t="n">
+        <v>99999</v>
+      </c>
+      <c r="C167" t="n">
+        <v>1</v>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>[3280]</t>
+        </is>
+      </c>
+      <c r="E167" t="n">
+        <v>3280</v>
+      </c>
+      <c r="F167" t="n">
+        <v>4103</v>
+      </c>
+      <c r="G167" t="n">
+        <v>0.7994</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>2604</v>
+      </c>
+      <c r="B168" t="n">
+        <v>24999</v>
+      </c>
+      <c r="C168" t="n">
+        <v>1</v>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>[3237]</t>
+        </is>
+      </c>
+      <c r="E168" t="n">
+        <v>3237</v>
+      </c>
+      <c r="F168" t="n">
+        <v>4037</v>
+      </c>
+      <c r="G168" t="n">
+        <v>0.8018</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>2605</v>
+      </c>
+      <c r="B169" t="n">
+        <v>349999</v>
+      </c>
+      <c r="C169" t="n">
+        <v>1</v>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>[3142]</t>
+        </is>
+      </c>
+      <c r="E169" t="n">
+        <v>3142</v>
+      </c>
+      <c r="F169" t="n">
+        <v>3947</v>
+      </c>
+      <c r="G169" t="n">
+        <v>0.796</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>2606</v>
+      </c>
+      <c r="B170" t="n">
+        <v>99999</v>
+      </c>
+      <c r="C170" t="n">
+        <v>1</v>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>[3129]</t>
+        </is>
+      </c>
+      <c r="E170" t="n">
+        <v>3129</v>
+      </c>
+      <c r="F170" t="n">
+        <v>3946</v>
+      </c>
+      <c r="G170" t="n">
+        <v>0.793</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>2607</v>
+      </c>
+      <c r="B171" t="n">
+        <v>24999</v>
+      </c>
+      <c r="C171" t="n">
+        <v>1</v>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>[3126]</t>
+        </is>
+      </c>
+      <c r="E171" t="n">
+        <v>3126</v>
+      </c>
+      <c r="F171" t="n">
+        <v>3891</v>
+      </c>
+      <c r="G171" t="n">
+        <v>0.8034</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>2608</v>
+      </c>
+      <c r="B172" t="n">
+        <v>49999</v>
+      </c>
+      <c r="C172" t="n">
+        <v>1</v>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>[3203]</t>
+        </is>
+      </c>
+      <c r="E172" t="n">
+        <v>3203</v>
+      </c>
+      <c r="F172" t="n">
+        <v>4030</v>
+      </c>
+      <c r="G172" t="n">
+        <v>0.7948</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>2609</v>
+      </c>
+      <c r="B173" t="n">
+        <v>1024999</v>
+      </c>
+      <c r="C173" t="n">
+        <v>1</v>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>[3240]</t>
+        </is>
+      </c>
+      <c r="E173" t="n">
+        <v>3240</v>
+      </c>
+      <c r="F173" t="n">
+        <v>4038</v>
+      </c>
+      <c r="G173" t="n">
+        <v>0.8024</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>2610</v>
+      </c>
+      <c r="B174" t="n">
+        <v>149999</v>
+      </c>
+      <c r="C174" t="n">
+        <v>1</v>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>[3302]</t>
+        </is>
+      </c>
+      <c r="E174" t="n">
+        <v>3302</v>
+      </c>
+      <c r="F174" t="n">
+        <v>4101</v>
+      </c>
+      <c r="G174" t="n">
+        <v>0.8052</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>2611</v>
+      </c>
+      <c r="B175" t="n">
+        <v>324999</v>
+      </c>
+      <c r="C175" t="n">
+        <v>1</v>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>[3269]</t>
+        </is>
+      </c>
+      <c r="E175" t="n">
+        <v>3269</v>
+      </c>
+      <c r="F175" t="n">
+        <v>4086</v>
+      </c>
+      <c r="G175" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>2612</v>
+      </c>
+      <c r="B176" t="n">
+        <v>49999</v>
+      </c>
+      <c r="C176" t="n">
+        <v>1</v>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>[3191]</t>
+        </is>
+      </c>
+      <c r="E176" t="n">
+        <v>3191</v>
+      </c>
+      <c r="F176" t="n">
+        <v>3986</v>
+      </c>
+      <c r="G176" t="n">
+        <v>0.8006</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>2613</v>
+      </c>
+      <c r="B177" t="n">
+        <v>99999</v>
+      </c>
+      <c r="C177" t="n">
+        <v>1</v>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>[3154]</t>
+        </is>
+      </c>
+      <c r="E177" t="n">
+        <v>3154</v>
+      </c>
+      <c r="F177" t="n">
+        <v>3936</v>
+      </c>
+      <c r="G177" t="n">
+        <v>0.8013</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>2614</v>
+      </c>
+      <c r="B178" t="n">
+        <v>49999</v>
+      </c>
+      <c r="C178" t="n">
+        <v>1</v>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>[3176]</t>
+        </is>
+      </c>
+      <c r="E178" t="n">
+        <v>3176</v>
+      </c>
+      <c r="F178" t="n">
+        <v>3971</v>
+      </c>
+      <c r="G178" t="n">
+        <v>0.7998</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>2615</v>
+      </c>
+      <c r="B179" t="n">
+        <v>49999</v>
+      </c>
+      <c r="C179" t="n">
+        <v>1</v>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>[3209]</t>
+        </is>
+      </c>
+      <c r="E179" t="n">
+        <v>3209</v>
+      </c>
+      <c r="F179" t="n">
+        <v>4007</v>
+      </c>
+      <c r="G179" t="n">
+        <v>0.8008</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>2616</v>
+      </c>
+      <c r="B180" t="n">
+        <v>199999</v>
+      </c>
+      <c r="C180" t="n">
+        <v>1</v>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>[3316]</t>
+        </is>
+      </c>
+      <c r="E180" t="n">
+        <v>3316</v>
+      </c>
+      <c r="F180" t="n">
+        <v>4080</v>
+      </c>
+      <c r="G180" t="n">
+        <v>0.8127</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>2617</v>
+      </c>
+      <c r="B181" t="n">
+        <v>49999</v>
+      </c>
+      <c r="C181" t="n">
+        <v>1</v>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>[3079]</t>
+        </is>
+      </c>
+      <c r="E181" t="n">
+        <v>3079</v>
+      </c>
+      <c r="F181" t="n">
+        <v>3918</v>
+      </c>
+      <c r="G181" t="n">
+        <v>0.7859</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="n">
+        <v>2618</v>
+      </c>
+      <c r="B182" t="n">
+        <v>274999</v>
+      </c>
+      <c r="C182" t="n">
+        <v>1</v>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>[3213]</t>
+        </is>
+      </c>
+      <c r="E182" t="n">
+        <v>3213</v>
+      </c>
+      <c r="F182" t="n">
+        <v>4012</v>
+      </c>
+      <c r="G182" t="n">
+        <v>0.8008</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="n">
+        <v>2619</v>
+      </c>
+      <c r="B183" t="n">
+        <v>99999</v>
+      </c>
+      <c r="C183" t="n">
+        <v>1</v>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>[3239]</t>
+        </is>
+      </c>
+      <c r="E183" t="n">
+        <v>3239</v>
+      </c>
+      <c r="F183" t="n">
+        <v>4015</v>
+      </c>
+      <c r="G183" t="n">
+        <v>0.8067</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="n">
+        <v>2620</v>
+      </c>
+      <c r="B184" t="n">
+        <v>99999</v>
+      </c>
+      <c r="C184" t="n">
+        <v>1</v>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>[3216]</t>
+        </is>
+      </c>
+      <c r="E184" t="n">
+        <v>3216</v>
+      </c>
+      <c r="F184" t="n">
+        <v>3971</v>
+      </c>
+      <c r="G184" t="n">
+        <v>0.8099</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="n">
+        <v>2621</v>
+      </c>
+      <c r="B185" t="n">
+        <v>74999</v>
+      </c>
+      <c r="C185" t="n">
+        <v>1</v>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>[3208]</t>
+        </is>
+      </c>
+      <c r="E185" t="n">
+        <v>3208</v>
+      </c>
+      <c r="F185" t="n">
+        <v>3990</v>
+      </c>
+      <c r="G185" t="n">
+        <v>0.804</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="n">
+        <v>2622</v>
+      </c>
+      <c r="B186" t="n">
+        <v>74999</v>
+      </c>
+      <c r="C186" t="n">
+        <v>1</v>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>[3170]</t>
+        </is>
+      </c>
+      <c r="E186" t="n">
+        <v>3170</v>
+      </c>
+      <c r="F186" t="n">
+        <v>3951</v>
+      </c>
+      <c r="G186" t="n">
+        <v>0.8023</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="n">
+        <v>2623</v>
+      </c>
+      <c r="B187" t="n">
+        <v>524999</v>
+      </c>
+      <c r="C187" t="n">
+        <v>1</v>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>[3234]</t>
+        </is>
+      </c>
+      <c r="E187" t="n">
+        <v>3234</v>
+      </c>
+      <c r="F187" t="n">
+        <v>4020</v>
+      </c>
+      <c r="G187" t="n">
+        <v>0.8045</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="n">
+        <v>2624</v>
+      </c>
+      <c r="B188" t="n">
+        <v>74999</v>
+      </c>
+      <c r="C188" t="n">
+        <v>1</v>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>[3251]</t>
+        </is>
+      </c>
+      <c r="E188" t="n">
+        <v>3251</v>
+      </c>
+      <c r="F188" t="n">
+        <v>4053</v>
+      </c>
+      <c r="G188" t="n">
+        <v>0.8021</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="n">
+        <v>2625</v>
+      </c>
+      <c r="B189" t="n">
+        <v>24999</v>
+      </c>
+      <c r="C189" t="n">
+        <v>1</v>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>[3140]</t>
+        </is>
+      </c>
+      <c r="E189" t="n">
+        <v>3140</v>
+      </c>
+      <c r="F189" t="n">
+        <v>3940</v>
+      </c>
+      <c r="G189" t="n">
+        <v>0.797</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="n">
+        <v>2626</v>
+      </c>
+      <c r="B190" t="n">
+        <v>49999</v>
+      </c>
+      <c r="C190" t="n">
+        <v>1</v>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>[3193]</t>
+        </is>
+      </c>
+      <c r="E190" t="n">
+        <v>3193</v>
+      </c>
+      <c r="F190" t="n">
+        <v>3984</v>
+      </c>
+      <c r="G190" t="n">
+        <v>0.8015</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="n">
+        <v>2627</v>
+      </c>
+      <c r="B191" t="n">
+        <v>74999</v>
+      </c>
+      <c r="C191" t="n">
+        <v>1</v>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>[3152]</t>
+        </is>
+      </c>
+      <c r="E191" t="n">
+        <v>3152</v>
+      </c>
+      <c r="F191" t="n">
+        <v>3961</v>
+      </c>
+      <c r="G191" t="n">
+        <v>0.7958</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="n">
+        <v>2628</v>
+      </c>
+      <c r="B192" t="n">
+        <v>24999</v>
+      </c>
+      <c r="C192" t="n">
+        <v>1</v>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>[3255]</t>
+        </is>
+      </c>
+      <c r="E192" t="n">
+        <v>3255</v>
+      </c>
+      <c r="F192" t="n">
+        <v>3996</v>
+      </c>
+      <c r="G192" t="n">
+        <v>0.8146</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="n">
+        <v>2629</v>
+      </c>
+      <c r="B193" t="n">
+        <v>774999</v>
+      </c>
+      <c r="C193" t="n">
+        <v>1</v>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>[3175]</t>
+        </is>
+      </c>
+      <c r="E193" t="n">
+        <v>3175</v>
+      </c>
+      <c r="F193" t="n">
+        <v>3909</v>
+      </c>
+      <c r="G193" t="n">
+        <v>0.8122</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="n">
+        <v>2630</v>
+      </c>
+      <c r="B194" t="n">
+        <v>74999</v>
+      </c>
+      <c r="C194" t="n">
+        <v>1</v>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>[3217]</t>
+        </is>
+      </c>
+      <c r="E194" t="n">
+        <v>3217</v>
+      </c>
+      <c r="F194" t="n">
+        <v>4038</v>
+      </c>
+      <c r="G194" t="n">
+        <v>0.7967</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="n">
+        <v>2631</v>
+      </c>
+      <c r="B195" t="n">
+        <v>449999</v>
+      </c>
+      <c r="C195" t="n">
+        <v>1</v>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>[3239]</t>
+        </is>
+      </c>
+      <c r="E195" t="n">
+        <v>3239</v>
+      </c>
+      <c r="F195" t="n">
+        <v>4055</v>
+      </c>
+      <c r="G195" t="n">
+        <v>0.7988</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="n">
+        <v>2632</v>
+      </c>
+      <c r="B196" t="n">
+        <v>49999</v>
+      </c>
+      <c r="C196" t="n">
+        <v>1</v>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>[3131]</t>
+        </is>
+      </c>
+      <c r="E196" t="n">
+        <v>3131</v>
+      </c>
+      <c r="F196" t="n">
+        <v>3981</v>
+      </c>
+      <c r="G196" t="n">
+        <v>0.7865</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="n">
+        <v>2633</v>
+      </c>
+      <c r="B197" t="n">
+        <v>99999</v>
+      </c>
+      <c r="C197" t="n">
+        <v>1</v>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>[3263]</t>
+        </is>
+      </c>
+      <c r="E197" t="n">
+        <v>3263</v>
+      </c>
+      <c r="F197" t="n">
+        <v>4066</v>
+      </c>
+      <c r="G197" t="n">
+        <v>0.8025</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="n">
+        <v>2634</v>
+      </c>
+      <c r="B198" t="n">
+        <v>924999</v>
+      </c>
+      <c r="C198" t="n">
+        <v>1</v>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>[3150]</t>
+        </is>
+      </c>
+      <c r="E198" t="n">
+        <v>3150</v>
+      </c>
+      <c r="F198" t="n">
+        <v>3960</v>
+      </c>
+      <c r="G198" t="n">
+        <v>0.7955</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="n">
+        <v>2635</v>
+      </c>
+      <c r="B199" t="n">
+        <v>24999</v>
+      </c>
+      <c r="C199" t="n">
+        <v>1</v>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>[3099]</t>
+        </is>
+      </c>
+      <c r="E199" t="n">
+        <v>3099</v>
+      </c>
+      <c r="F199" t="n">
+        <v>3924</v>
+      </c>
+      <c r="G199" t="n">
+        <v>0.7897999999999999</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="n">
+        <v>2636</v>
+      </c>
+      <c r="B200" t="n">
+        <v>24999</v>
+      </c>
+      <c r="C200" t="n">
+        <v>1</v>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>[3211]</t>
+        </is>
+      </c>
+      <c r="E200" t="n">
+        <v>3211</v>
+      </c>
+      <c r="F200" t="n">
+        <v>4055</v>
+      </c>
+      <c r="G200" t="n">
+        <v>0.7919</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="n">
+        <v>2637</v>
+      </c>
+      <c r="B201" t="n">
+        <v>149999</v>
+      </c>
+      <c r="C201" t="n">
+        <v>1</v>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>[3228]</t>
+        </is>
+      </c>
+      <c r="E201" t="n">
+        <v>3228</v>
+      </c>
+      <c r="F201" t="n">
+        <v>3947</v>
+      </c>
+      <c r="G201" t="n">
+        <v>0.8178</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>